<commit_message>
final addition of data
- added UR for analysis
- added different tax values from FED (for standardized methods)
- create an overlap of tax incidence in CA
</commit_message>
<xml_diff>
--- a/code_data/inputs/CA_Exports_Imports-onetable.xlsx
+++ b/code_data/inputs/CA_Exports_Imports-onetable.xlsx
@@ -1,25 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/allegrasaggese/Documents/GitHub/econ221_fall2025/code_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/allegrasaggese/Documents/GitHub/econ221_fall2025/code_data/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A663575-A951-A24D-A5EE-A0D0CCCBF50E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB43AD30-D39E-894F-9E45-F57DD28E4527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="24360" windowHeight="17020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="24360" windowHeight="17020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="CA Exports Imports Annual" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Villalpando, Karina - Personal View" guid="{6EEAC7C3-6FD8-4EC1-902D-EEDDA6398FAC}" mergeInterval="0" personalView="1" xWindow="1210" yWindow="40" windowWidth="971" windowHeight="1113" activeSheetId="1"/>
     <customWorkbookView name="Karina Villalpando - Personal View" guid="{DD2A8D8A-D13E-4C74-90E3-719DE4611D5A}" mergeInterval="0" personalView="1" maximized="1" xWindow="-4" yWindow="-4" windowWidth="1370" windowHeight="814" activeSheetId="1"/>
-    <customWorkbookView name="Villalpando, Karina - Personal View" guid="{6EEAC7C3-6FD8-4EC1-902D-EEDDA6398FAC}" mergeInterval="0" personalView="1" xWindow="1210" yWindow="40" windowWidth="971" windowHeight="1113" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,64 +40,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="14">
-  <si>
-    <t>EXPORT AND IMPORT TOTALS FOR CALIFORNIA</t>
-  </si>
-  <si>
-    <t>(Values are in millions of U.S. dollars)</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Exports</t>
-  </si>
-  <si>
-    <t>% change</t>
-  </si>
-  <si>
-    <t>Imports</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOTAL </t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>State Imports are State of Destination, meaning the state where the goods will end their trade journey. (Annual from 2008).</t>
-  </si>
-  <si>
-    <t>Source: U.S. Census Bureau, Foreign Trade Division.</t>
-  </si>
-  <si>
-    <t>Updated: February 2024.</t>
-  </si>
-  <si>
-    <t>Next update: February 2025.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>year</t>
   </si>
   <si>
     <t>exports_mill_dollars</t>
   </si>
+  <si>
+    <t>imports_mill_dollars</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="7">
+  <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0_);\(#,##0.0\)"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="0.0_);[Red]\(0.0\)"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -227,32 +187,13 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -430,12 +371,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -564,7 +499,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -608,85 +543,32 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="19" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="19" fillId="0" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="19" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="37" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="37" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="37" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="37" fontId="22" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="22" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="10" xfId="44" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="19" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="0" borderId="10" xfId="44" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
@@ -714,8 +596,7 @@
     <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Comma" xfId="43" builtinId="3"/>
-    <cellStyle name="Currency" xfId="44" builtinId="4"/>
+    <cellStyle name="Currency" xfId="43" builtinId="4"/>
     <cellStyle name="Explanatory Text" xfId="28" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Good" xfId="29" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="30" builtinId="16" customBuiltin="1"/>
@@ -1100,822 +981,259 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L29"/>
-  <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:B25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="12.75" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="7" width="14.6640625" customWidth="1"/>
-    <col min="8" max="12" width="0" hidden="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.1640625" hidden="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-    </row>
-    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-    </row>
-    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.15">
-      <c r="A3" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
-        <v>2002</v>
-      </c>
-      <c r="B4" s="3">
-        <v>92177.510781999998</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
-        <v>2003</v>
-      </c>
-      <c r="B5" s="4">
-        <v>93906.331502999994</v>
-      </c>
-      <c r="C5" s="14">
-        <v>1.8755341800112735</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
-        <v>2004</v>
-      </c>
-      <c r="B6" s="4">
-        <v>110143.572288</v>
-      </c>
-      <c r="C6" s="14">
-        <v>17.290890321363772</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
-        <v>2005</v>
-      </c>
-      <c r="B7" s="4">
-        <v>116689.90180399999</v>
-      </c>
-      <c r="C7" s="14">
-        <v>5.9434512427859687</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
-        <v>2006</v>
-      </c>
-      <c r="B8" s="4">
-        <v>127770.79381</v>
-      </c>
-      <c r="C8" s="14">
-        <v>9.4960162230766088</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
-        <v>2007</v>
-      </c>
-      <c r="B9" s="4">
-        <v>134318.90676099999</v>
-      </c>
-      <c r="C9" s="14">
-        <v>5.1248902474044788</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
-        <v>2008</v>
-      </c>
-      <c r="B10" s="4">
-        <v>144805.748349</v>
-      </c>
-      <c r="C10" s="14">
-        <v>7.8074202961313066</v>
-      </c>
-      <c r="D10" s="3">
-        <v>348268.55651700002</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="3">
-        <v>493074.30486600002</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
-        <v>2009</v>
-      </c>
-      <c r="B11" s="4">
-        <v>120079.965765</v>
-      </c>
-      <c r="C11" s="14">
-        <v>-17.075138843526961</v>
-      </c>
-      <c r="D11" s="5">
-        <v>270414.46974700002</v>
-      </c>
-      <c r="E11" s="14">
-        <v>-22.354612643935223</v>
-      </c>
-      <c r="F11" s="5">
-        <v>390494.435512</v>
-      </c>
-      <c r="G11" s="14">
-        <v>-20.804140135000047</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
-        <v>2010</v>
-      </c>
-      <c r="B12" s="4">
-        <v>143208.226608</v>
-      </c>
-      <c r="C12" s="14">
-        <v>19.260715720274835</v>
-      </c>
-      <c r="D12" s="5">
-        <v>327265.73167499999</v>
-      </c>
-      <c r="E12" s="14">
-        <v>21.023749942519743</v>
-      </c>
-      <c r="F12" s="5">
-        <v>470473.95828299999</v>
-      </c>
-      <c r="G12" s="14">
-        <v>20.481603704834917</v>
-      </c>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
-        <v>2011</v>
-      </c>
-      <c r="B13" s="4">
-        <v>159421.39388600001</v>
-      </c>
-      <c r="C13" s="14">
-        <v>11.321393792816025</v>
-      </c>
-      <c r="D13" s="5">
-        <v>351597.45800599997</v>
-      </c>
-      <c r="E13" s="14">
-        <v>7.4348530799317691</v>
-      </c>
-      <c r="F13" s="5">
-        <v>511018.85189199995</v>
-      </c>
-      <c r="G13" s="14">
-        <v>8.6178826468884751</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
-        <v>2012</v>
-      </c>
-      <c r="B14" s="4">
-        <v>161757.31064800001</v>
-      </c>
-      <c r="C14" s="14">
-        <v>1.4652467307307404</v>
-      </c>
-      <c r="D14" s="5">
-        <v>376487.23414299998</v>
-      </c>
-      <c r="E14" s="14">
-        <v>7.0790546320091075</v>
-      </c>
-      <c r="F14" s="5">
-        <v>538244.54479099996</v>
-      </c>
-      <c r="G14" s="14">
-        <v>5.3277276950154384</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <v>2013</v>
-      </c>
-      <c r="B15" s="4">
-        <v>168191.55155999999</v>
-      </c>
-      <c r="C15" s="14">
-        <v>3.9777125906856448</v>
-      </c>
-      <c r="D15" s="5">
-        <v>381068.94531400001</v>
-      </c>
-      <c r="E15" s="14">
-        <v>1.2169632209255044</v>
-      </c>
-      <c r="F15" s="5">
-        <v>549260.49687399995</v>
-      </c>
-      <c r="G15" s="14">
-        <v>2.0466444462112321</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
-        <v>2014</v>
-      </c>
-      <c r="B16" s="4">
-        <v>173868.58786199999</v>
-      </c>
-      <c r="C16" s="14">
-        <v>3.3753397535992047</v>
-      </c>
-      <c r="D16" s="5">
-        <v>403808.03783599997</v>
-      </c>
-      <c r="E16" s="14">
-        <v>5.9671859388234827</v>
-      </c>
-      <c r="F16" s="5">
-        <v>577676.62569799996</v>
-      </c>
-      <c r="G16" s="14">
-        <v>5.1735249459453847</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
-        <v>2015</v>
-      </c>
-      <c r="B17" s="4">
-        <v>165360.37779999999</v>
-      </c>
-      <c r="C17" s="14">
-        <v>-4.8934716538636565</v>
-      </c>
-      <c r="D17" s="5">
-        <v>408337.164437</v>
-      </c>
-      <c r="E17" s="14">
-        <v>1.1216038752649649</v>
-      </c>
-      <c r="F17" s="5">
-        <v>573697.54223699996</v>
-      </c>
-      <c r="G17" s="14">
-        <v>-0.68880811235734196</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
-        <v>2016</v>
-      </c>
-      <c r="B18" s="4">
-        <v>163260.62358499999</v>
-      </c>
-      <c r="C18" s="14">
-        <v>-1.2698049211883222</v>
-      </c>
-      <c r="D18" s="5">
-        <v>410062.132408</v>
-      </c>
-      <c r="E18" s="14">
-        <v>0.42243717232506306</v>
-      </c>
-      <c r="F18" s="5">
-        <v>573322.755993</v>
-      </c>
-      <c r="G18" s="14">
-        <v>-6.5328194110536586E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
-        <v>2017</v>
-      </c>
-      <c r="B19" s="7">
-        <v>171920.43058499999</v>
-      </c>
-      <c r="C19" s="14">
-        <v>5.3042839172370071</v>
-      </c>
-      <c r="D19" s="7">
-        <v>440223.19405200001</v>
-      </c>
-      <c r="E19" s="14">
-        <v>7.3552418671009034</v>
-      </c>
-      <c r="F19" s="5">
-        <v>612143.62463700003</v>
-      </c>
-      <c r="G19" s="14">
-        <v>6.7712066612046318</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
-        <v>2018</v>
-      </c>
-      <c r="B20" s="7">
-        <v>178175.23564699999</v>
-      </c>
-      <c r="C20" s="14">
-        <v>3.638197648014585</v>
-      </c>
-      <c r="D20" s="7">
-        <v>440198.62990900001</v>
-      </c>
-      <c r="E20" s="14">
-        <v>-5.5799293022018581E-3</v>
-      </c>
-      <c r="F20" s="5">
-        <v>618373.86555600003</v>
-      </c>
-      <c r="G20" s="14">
-        <v>1.0177743699764097</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
-        <v>2019</v>
-      </c>
-      <c r="B21" s="7">
-        <v>173754.50772699999</v>
-      </c>
-      <c r="C21" s="14">
-        <v>-2.4811124306625465</v>
-      </c>
-      <c r="D21" s="7">
-        <v>407516.155058</v>
-      </c>
-      <c r="E21" s="14">
-        <v>-7.424483546838001</v>
-      </c>
-      <c r="F21" s="5">
-        <v>581270.66278499993</v>
-      </c>
-      <c r="G21" s="14">
-        <v>-6.0001246555980163</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
-        <v>2020</v>
-      </c>
-      <c r="B22" s="7">
-        <v>155919.092901</v>
-      </c>
-      <c r="C22" s="14">
-        <v>-10.26472064484375</v>
-      </c>
-      <c r="D22" s="7">
-        <v>395290.85595100001</v>
-      </c>
-      <c r="E22" s="14">
-        <v>-2.9999544693534941</v>
-      </c>
-      <c r="F22" s="5">
-        <v>551209.94885200006</v>
-      </c>
-      <c r="G22" s="14">
-        <v>-5.1715518875444673</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
-        <v>2021</v>
-      </c>
-      <c r="B23" s="7">
-        <v>174859.93087000001</v>
-      </c>
-      <c r="C23" s="14">
-        <v>12.147863110662405</v>
-      </c>
-      <c r="D23" s="7">
-        <v>469807.84635000001</v>
-      </c>
-      <c r="E23" s="14">
-        <v>18.851179903902725</v>
-      </c>
-      <c r="F23" s="5">
-        <v>644667.77722000005</v>
-      </c>
-      <c r="G23" s="14">
-        <v>16.955032934845192</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
-        <v>2022</v>
-      </c>
-      <c r="B24" s="7">
-        <v>186238.29135099999</v>
-      </c>
-      <c r="C24" s="14">
-        <v>6.5071285481973939</v>
-      </c>
-      <c r="D24" s="7">
-        <v>508724.56609600002</v>
-      </c>
-      <c r="E24" s="14">
-        <v>8.2835397595738769</v>
-      </c>
-      <c r="F24" s="5">
-        <v>694962.85744699999</v>
-      </c>
-      <c r="G24" s="14">
-        <v>7.8017053130664316</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="8">
-        <v>2023</v>
-      </c>
-      <c r="B25" s="9">
-        <v>178717.23368199999</v>
-      </c>
-      <c r="C25" s="15">
-        <v>-4.0384056438883427</v>
-      </c>
-      <c r="D25" s="9">
-        <v>449484.91996299999</v>
-      </c>
-      <c r="E25" s="15">
-        <v>-11.644738642682551</v>
-      </c>
-      <c r="F25" s="10">
-        <v>628202.15364499995</v>
-      </c>
-      <c r="G25" s="15">
-        <v>-9.6063700508039584</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="21"/>
-    </row>
-    <row r="27" spans="1:7" s="22" customFormat="1" ht="12" x14ac:dyDescent="0.15">
-      <c r="A27" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-    </row>
-    <row r="28" spans="1:7" s="22" customFormat="1" ht="12" x14ac:dyDescent="0.15">
-      <c r="A28" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="23"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-    </row>
-    <row r="29" spans="1:7" s="22" customFormat="1" ht="12" x14ac:dyDescent="0.15">
-      <c r="A29" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="21"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71E2F178-45D2-7140-BE87-3864477FE9BA}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="27" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="31">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
         <v>2002</v>
       </c>
-      <c r="B2" s="28">
+      <c r="B2" s="2">
         <v>92177.510781999998</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="31">
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
         <v>2003</v>
       </c>
-      <c r="B3" s="28">
+      <c r="B3" s="2">
         <v>93906.331502999994</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="31">
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
         <v>2004</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="2">
         <v>110143.572288</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="31">
+      <c r="C4" s="7"/>
+    </row>
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
         <v>2005</v>
       </c>
-      <c r="B5" s="28">
+      <c r="B5" s="2">
         <v>116689.90180399999</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="31">
+      <c r="C5" s="7"/>
+    </row>
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
         <v>2006</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B6" s="2">
         <v>127770.79381</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="31">
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
         <v>2007</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="2">
         <v>134318.90676099999</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="31">
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
         <v>2008</v>
       </c>
-      <c r="B8" s="28">
+      <c r="B8" s="2">
         <v>144805.748349</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="31">
+      <c r="C8" s="8">
+        <v>348269</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
         <v>2009</v>
       </c>
-      <c r="B9" s="28">
+      <c r="B9" s="2">
         <v>120079.965765</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="31">
+      <c r="C9" s="8">
+        <v>270414</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
         <v>2010</v>
       </c>
-      <c r="B10" s="28">
+      <c r="B10" s="2">
         <v>143208.226608</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="31">
+      <c r="C10" s="8">
+        <v>327266</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
         <v>2011</v>
       </c>
-      <c r="B11" s="28">
+      <c r="B11" s="2">
         <v>159421.39388600001</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="31">
+      <c r="C11" s="8">
+        <v>351597</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
         <v>2012</v>
       </c>
-      <c r="B12" s="28">
+      <c r="B12" s="2">
         <v>161757.31064800001</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="31">
+      <c r="C12" s="8">
+        <v>376487</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
         <v>2013</v>
       </c>
-      <c r="B13" s="28">
+      <c r="B13" s="2">
         <v>168191.55155999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="31">
+      <c r="C13" s="8">
+        <v>381069</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
         <v>2014</v>
       </c>
-      <c r="B14" s="28">
+      <c r="B14" s="2">
         <v>173868.58786199999</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="31">
+      <c r="C14" s="8">
+        <v>403808</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
         <v>2015</v>
       </c>
-      <c r="B15" s="28">
+      <c r="B15" s="2">
         <v>165360.37779999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="31">
+      <c r="C15" s="8">
+        <v>408337</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
         <v>2016</v>
       </c>
-      <c r="B16" s="28">
+      <c r="B16" s="2">
         <v>163260.62358499999</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="31">
+      <c r="C16" s="8">
+        <v>410062</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
         <v>2017</v>
       </c>
-      <c r="B17" s="29">
+      <c r="B17" s="3">
         <v>171920.43058499999</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="31">
+      <c r="C17" s="9">
+        <v>440223</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
         <v>2018</v>
       </c>
-      <c r="B18" s="29">
+      <c r="B18" s="3">
         <v>178175.23564699999</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="31">
+      <c r="C18" s="9">
+        <v>440199</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
         <v>2019</v>
       </c>
-      <c r="B19" s="29">
+      <c r="B19" s="3">
         <v>173754.50772699999</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="31">
+      <c r="C19" s="9">
+        <v>407516</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
         <v>2020</v>
       </c>
-      <c r="B20" s="29">
+      <c r="B20" s="3">
         <v>155919.092901</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="31">
+      <c r="C20" s="9">
+        <v>395291</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="5">
         <v>2021</v>
       </c>
-      <c r="B21" s="29">
+      <c r="B21" s="3">
         <v>174859.93087000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="31">
+      <c r="C21" s="9">
+        <v>469808</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="5">
         <v>2022</v>
       </c>
-      <c r="B22" s="29">
+      <c r="B22" s="3">
         <v>186238.29135099999</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="32">
+      <c r="C22" s="9">
+        <v>508725</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="6">
         <v>2023</v>
       </c>
-      <c r="B23" s="30">
+      <c r="B23" s="4">
         <v>178717.23368199999</v>
+      </c>
+      <c r="C23" s="10">
+        <v>449485</v>
       </c>
     </row>
   </sheetData>
@@ -1924,28 +1242,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="50b4d822-f145-40b1-b502-720eef342d4b" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4ca643c4-7cca-4cf7-9b44-d1a48358ecdb">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100133903503F928A40A5C7040A15395DCD" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="17c0b1408c4bddba4a326b4ac96a64fa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4ca643c4-7cca-4cf7-9b44-d1a48358ecdb" xmlns:ns3="50b4d822-f145-40b1-b502-720eef342d4b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="22a005c68d502a2d0a7d1126f2e9c260" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2191,27 +1487,29 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4FA0FB38-362A-485A-A86F-693D94A1ACB3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="50b4d822-f145-40b1-b502-720eef342d4b"/>
-    <ds:schemaRef ds:uri="4ca643c4-7cca-4cf7-9b44-d1a48358ecdb"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99696D85-630E-4DE9-9743-2124237515A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="50b4d822-f145-40b1-b502-720eef342d4b" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4ca643c4-7cca-4cf7-9b44-d1a48358ecdb">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB33EAF2-D161-44E2-BD8D-94088858D1C5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2229,4 +1527,24 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99696D85-630E-4DE9-9743-2124237515A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4FA0FB38-362A-485A-A86F-693D94A1ACB3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="50b4d822-f145-40b1-b502-720eef342d4b"/>
+    <ds:schemaRef ds:uri="4ca643c4-7cca-4cf7-9b44-d1a48358ecdb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>